<commit_message>
filtro + modifica generatore excel
</commit_message>
<xml_diff>
--- a/BE/persons.xlsx
+++ b/BE/persons.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,39 +425,39 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="str">
-        <v>Leo</v>
+        <v>Edo</v>
       </c>
       <c r="C2" s="1">
-        <v>45061.76314018518</v>
+        <v>45061.763309236114</v>
       </c>
       <c r="D2" t="str">
         <v>rich</v>
       </c>
       <c r="E2" t="str">
-        <v>Leo</v>
+        <v>Edo</v>
       </c>
       <c r="F2" t="str">
-        <v>USER</v>
+        <v>ADMIN</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <v>Edo</v>
+        <v>Ettore</v>
       </c>
       <c r="C3" s="1">
-        <v>45061.763309236114</v>
+        <v>45069.87578456019</v>
       </c>
       <c r="D3" t="str">
         <v>rich</v>
       </c>
       <c r="E3" t="str">
-        <v>Edo</v>
+        <v>Ettore</v>
       </c>
       <c r="F3" t="str">
         <v>ADMIN</v>
@@ -465,27 +465,47 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="str">
-        <v>Ettore</v>
+        <v>Giacomo</v>
       </c>
       <c r="C4" s="1">
-        <v>45069.87578456019</v>
+        <v>45070.984361331015</v>
       </c>
       <c r="D4" t="str">
         <v>rich</v>
       </c>
       <c r="E4" t="str">
-        <v>Ettore</v>
+        <v>Giacomo</v>
       </c>
       <c r="F4" t="str">
+        <v>ADMIN</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Fabrizio</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45070.9851908912</v>
+      </c>
+      <c r="D5" t="str">
+        <v>rich</v>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
         <v>ADMIN</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>